<commit_message>
comment removed from face_recog
</commit_message>
<xml_diff>
--- a/attendance_record.xlsx
+++ b/attendance_record.xlsx
@@ -455,11 +455,11 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-12-08 13:11:23</t>
+          <t>2024-12-13 11:09:13</t>
         </is>
       </c>
     </row>

</xml_diff>